<commit_message>
definitions superceded by code modules
</commit_message>
<xml_diff>
--- a/SIA IDI Definitions Library Catalogue.xlsx
+++ b/SIA IDI Definitions Library Catalogue.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NotBackedUp\github_migration\sia\definitions_library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NotBackedUp\git\definitions_library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309D4F5E-4D57-458D-BBC1-19985A1598FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C9A97F-4BFE-4BAF-888B-4AA04412D246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="529">
   <si>
     <t>Domain</t>
   </si>
@@ -1997,6 +1997,18 @@
   </si>
   <si>
     <t>The definitions provided in this library were determined by the Social Investment Agency (previously Social Wellbeing Agency) to be suitable in the context of a specific project. Whether or not these definitions are suitable for other projects depends on the context of those projects. Researchers using definitions from this library will need to determine for themselves to what extent the definitions provided here are suitable for reuse in their projects. While the Agency provides this library as a resource to support IDI research, it provides no guarantee that these definitions are fit for reuse.</t>
+  </si>
+  <si>
+    <t>Partial</t>
+  </si>
+  <si>
+    <t>Driver licence code module now available</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Code module now available</t>
   </si>
 </sst>
 </file>
@@ -2503,9 +2515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2595,7 +2605,7 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>163</v>
+        <v>527</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -2953,7 +2963,7 @@
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4" t="s">
-        <v>163</v>
+        <v>527</v>
       </c>
       <c r="I17" s="4"/>
     </row>
@@ -3028,7 +3038,7 @@
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4" t="s">
-        <v>163</v>
+        <v>527</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>402</v>
@@ -4835,7 +4845,7 @@
         <v>5</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>163</v>
+        <v>527</v>
       </c>
       <c r="I91" s="4" t="s">
         <v>116</v>
@@ -4864,7 +4874,7 @@
         <v>5</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>163</v>
+        <v>527</v>
       </c>
       <c r="I92" s="4" t="s">
         <v>120</v>
@@ -4968,9 +4978,11 @@
       </c>
       <c r="G96" s="4"/>
       <c r="H96" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="I96" s="4"/>
+        <v>527</v>
+      </c>
+      <c r="I96" s="4" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
@@ -4993,9 +5005,11 @@
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="I97" s="4"/>
+        <v>527</v>
+      </c>
+      <c r="I97" s="4" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="98" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
@@ -5043,9 +5057,11 @@
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="I99" s="4"/>
+        <v>525</v>
+      </c>
+      <c r="I99" s="4" t="s">
+        <v>526</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I99" xr:uid="{00000000-0001-0000-0000-000000000000}">

</xml_diff>